<commit_message>
Actualización de archivos y reorganización del proyecto
</commit_message>
<xml_diff>
--- a/resultados_facturas.xlsx
+++ b/resultados_facturas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,17 +478,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>20555841095</t>
+          <t>20600212568</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E001-57</t>
+          <t>E001-2352</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>07/07/2023</t>
+          <t>10/01/2023</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -498,39 +498,40 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>No encontrado</t>
+          <t>Contado
+1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>0.00</t>
+          <t>59.00</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t xml:space="preserve">GM INGENIEROS Y CONSULTORES </t>
+          <t>MS SERVCOM S.R.L.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>AV. VENEZUELA 625 DPTO. 1013 CND. EDIFICIO ROCE FRENTE AL METRO DE ALFONSO UGARTE 625 BREÑA - LIMA - LIMA</t>
+          <t>PRO. LAS CEREZAS URB. SURCO MZA. C LOTE. 10 SANTIAGO DE SURCO - LIMA - LIMA</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>20555841095</t>
+          <t>10321225972</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>E001-226</t>
+          <t>E001-322</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>03/07/2023</t>
+          <t>14/01/2023</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -540,23 +541,152 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Crédito
+          <t>Contado
 1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>31,202.74</t>
+          <t>50.00</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>GM INGENIEROS Y CONSULTORES</t>
+          <t>HOSTAL VENUS</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>AV. VENEZUELA 625 CND. EDIFICIO ROCE DPTO. 1013 FRENTE AL METRO DE ALFONSO UGARTE BREÑA - LIMA - LIMA FACTURA ELECTRONICA</t>
+          <t>CAL. GRAU HABITAC. URBANO II MZA. H LOTE. 14 NRO. 353 ESPALDAS DE LA PLAZA DE ARMAS HUARMEY - HUARMEY - ANCASH</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>10464300398</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>E001-4274</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>16/02/2023</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Contado
+1</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>16.50</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>FERRETERIA EL RAPIDO</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>JR. WASHINGTON 1103 LIMA - LIMA - LIMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>10706290741</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>E001-46</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>27/02/2023</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Contado
+1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>25.00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>VALDIVIA ROBLES SARA</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>JR. CAMANA 1184 INT. 05 LIMA - LIMA - LIMA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>10411214732</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>E001-94</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>15/02/2023</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>SOLES</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Contado
+1</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>49.91</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>MULTISERVICIOS AMAZONAS</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>AV. VENEZUELA 625 CND. EDIFICIO ROCE DPTO. 1013 FRENTE AL METRO DE ALFONSO UGARTE LIMA-LIMA-BREÑA</t>
         </is>
       </c>
     </row>

</xml_diff>